<commit_message>
PSP sheet, PMP sheet update
</commit_message>
<xml_diff>
--- a/PSP_Sheet.xlsx
+++ b/PSP_Sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leejunki/Desktop/19년 2학기/빅데이터종합설계/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leejunki/Bigdata_Capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A284010-9B36-7A4F-9F48-4B13B7387F77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B46578-2FF9-7048-8AA0-E30CA6C968A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -609,7 +609,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Table C16  Time Recording Log</t>
   </si>
@@ -680,6 +680,66 @@
     <t>github repository 생성 및 collaborators 추가</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>9월 26일</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>월</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 25</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>주제 수정 및 개선사항 점검</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>기존 논문 및 사례 조사</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>9월 30일</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>해외 및 국내 사례 조사, 기상청 기존 API 분석</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>10월 1일</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>서베이 발표 및 GUI 디자인 회의, 요약본 요청</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -689,7 +749,7 @@
     <numFmt numFmtId="176" formatCode="m&quot;월&quot;\ d&quot;일&quot;;@"/>
     <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -749,6 +809,12 @@
     <font>
       <sz val="10"/>
       <name val="돋움"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Malgun Gothic"/>
       <family val="2"/>
       <charset val="129"/>
     </font>
@@ -1276,7 +1342,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
@@ -1415,36 +1481,84 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1">
-      <c r="A10" s="14"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="4"/>
+      <c r="A10" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="9">
+        <v>0</v>
+      </c>
+      <c r="E10" s="16">
+        <v>120</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1">
-      <c r="A11" s="15"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="5"/>
+      <c r="A11" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="D11" s="10">
+        <v>0</v>
+      </c>
+      <c r="E11" s="17">
+        <v>75</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1">
-      <c r="A12" s="14"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="4"/>
+      <c r="A12" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D12" s="9">
+        <v>0</v>
+      </c>
+      <c r="E12" s="16">
+        <v>240</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1">
-      <c r="A13" s="14"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="4"/>
+      <c r="A13" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0</v>
+      </c>
+      <c r="E13" s="16">
+        <v>75</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="14"/>

</xml_diff>

<commit_message>
update PMP/PSP with Suin's
</commit_message>
<xml_diff>
--- a/PSP_Sheet.xlsx
+++ b/PSP_Sheet.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leejunki/Bigdata_Capstone/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Bigdata_Capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B46578-2FF9-7048-8AA0-E30CA6C968A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE850EE2-B21B-40EC-B185-302987568676}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="432" yWindow="0" windowWidth="22608" windowHeight="12384" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="작성자명" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="이준기" sheetId="1" r:id="rId1"/>
+    <sheet name="김수인" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
@@ -608,8 +608,574 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{5E766E14-882C-4EB4-B28D-E29C026D039B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Soojin Park:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>작업하다가</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>중간에</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> interrupt</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>가</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>걸린</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>시간을</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>뜻함</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{A2587C53-4B11-4EC1-B556-E6FC7E92B5C7}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Soojin Park:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
+            <charset val="129"/>
+          </rPr>
+          <t>중간에</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> interrupt </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
+            <charset val="129"/>
+          </rPr>
+          <t>걸린</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
+            <charset val="129"/>
+          </rPr>
+          <t>시간</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
+            <charset val="129"/>
+          </rPr>
+          <t>포함</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
+            <charset val="129"/>
+          </rPr>
+          <t>작업시간</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>. 10</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
+            <charset val="129"/>
+          </rPr>
+          <t>분</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
+            <charset val="129"/>
+          </rPr>
+          <t>단위로</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
+            <charset val="129"/>
+          </rPr>
+          <t>작성</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="2"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{AFD999F1-BDBC-4F89-95BD-0410B3853DAE}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Soojin Park:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>원래</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Phase</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>를</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>기술하지만</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">, </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>우리는</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>관련된</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Activity</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>가</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>뭔지를</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>기술하도록</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>함</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">. </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>성혜가</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>작성하는</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Test Case </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>정도의</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Granulity</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>로</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>작성할</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>것</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="47">
   <si>
     <t>Table C16  Time Recording Log</t>
   </si>
@@ -738,6 +1304,823 @@
   </si>
   <si>
     <t>서베이 발표 및 GUI 디자인 회의, 요약본 요청</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>작성자명</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> : 김수인</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>월 19일</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>주제</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>선정</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>및</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> skeleton code </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>작성자</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>선정</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>월 20일</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Mission_0_template</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>작성 및 주제 구체화</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>월 23일</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>차</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>회의록</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>작성</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>월</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 25</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>주제 수정 및 개선사항 점검</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">차 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>회의록</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>작성</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>월 30일</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>해외</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>및</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>국내</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>사례</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>조사</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>기상청</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>기존</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> API </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>분석</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, PPT </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>작성</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>월 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PPT </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>추가</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>작성</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>및</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>발표</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>초본</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>작성</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>월 1일</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>서베이 발표 및 GUI 디자인 회의, 요약본 요청</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>월</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 27</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PPT </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>추가</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>작성</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>및</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>발표</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>초본</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>작성</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>월</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 27</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2차 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>회의록</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>작성</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>10월 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일</t>
+    </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -749,7 +2132,7 @@
     <numFmt numFmtId="176" formatCode="m&quot;월&quot;\ d&quot;일&quot;;@"/>
     <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -816,6 +2199,23 @@
       <sz val="10"/>
       <name val="Malgun Gothic"/>
       <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
       <charset val="129"/>
     </font>
   </fonts>
@@ -895,7 +2295,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
@@ -956,6 +2356,34 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="열어본 하이퍼링크" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -1341,20 +2769,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="11.5" style="8" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" style="8" customWidth="1"/>
     <col min="5" max="5" width="9.6640625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="46.5" customWidth="1"/>
+    <col min="6" max="6" width="46.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="11.75" customHeight="1">
+    <row r="1" spans="1:6" ht="11.7" customHeight="1">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1366,10 +2794,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="11.75" customHeight="1">
+    <row r="2" spans="1:6" ht="11.7" customHeight="1">
       <c r="A2" s="20"/>
     </row>
-    <row r="3" spans="1:6" ht="11.75" customHeight="1">
+    <row r="3" spans="1:6" ht="11.7" customHeight="1">
       <c r="A3" s="19" t="s">
         <v>8</v>
       </c>
@@ -1379,8 +2807,8 @@
       </c>
       <c r="E3"/>
     </row>
-    <row r="4" spans="1:6" ht="11.75" customHeight="1"/>
-    <row r="5" spans="1:6" s="11" customFormat="1" ht="28">
+    <row r="4" spans="1:6" ht="11.7" customHeight="1"/>
+    <row r="5" spans="1:6" s="11" customFormat="1" ht="26.4">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
@@ -1777,7 +3205,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1794,7 +3222,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1811,7 +3239,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1828,7 +3256,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1845,7 +3273,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1862,7 +3290,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1879,7 +3307,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1891,19 +3319,279 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="20"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:11" ht="13.8">
+      <c r="A3" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="D3" s="19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:11" ht="26.4">
+      <c r="A5" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
+    </row>
+    <row r="6" spans="1:11" ht="13.8">
+      <c r="A6" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="C6" s="31">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="D6" s="32">
+        <v>0</v>
+      </c>
+      <c r="E6" s="33">
+        <v>75</v>
+      </c>
+      <c r="F6" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="37">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C7" s="37">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D7" s="38">
+        <v>0</v>
+      </c>
+      <c r="E7" s="39">
+        <v>60</v>
+      </c>
+      <c r="F7" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+    </row>
+    <row r="8" spans="1:11" ht="13.8">
+      <c r="A8" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="37">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C8" s="37">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D8" s="38">
+        <v>0</v>
+      </c>
+      <c r="E8" s="39">
+        <v>30</v>
+      </c>
+      <c r="F8" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
+    </row>
+    <row r="9" spans="1:11" ht="15.6">
+      <c r="A9" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="41">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C9" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="42">
+        <v>0</v>
+      </c>
+      <c r="E9" s="43">
+        <v>120</v>
+      </c>
+      <c r="F9" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="35"/>
+    </row>
+    <row r="10" spans="1:11" ht="15.6">
+      <c r="A10" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="41">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C10" s="41">
+        <v>0.1875</v>
+      </c>
+      <c r="D10" s="42">
+        <v>0</v>
+      </c>
+      <c r="E10" s="43">
+        <v>30</v>
+      </c>
+      <c r="F10" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="35"/>
+    </row>
+    <row r="11" spans="1:11" ht="15.6">
+      <c r="A11" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="41">
+        <v>0.75</v>
+      </c>
+      <c r="C11" s="41">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D11" s="42">
+        <v>0</v>
+      </c>
+      <c r="E11" s="43">
+        <v>240</v>
+      </c>
+      <c r="F11" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35"/>
+    </row>
+    <row r="12" spans="1:11" ht="13.8">
+      <c r="A12" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="41">
+        <v>0.4375</v>
+      </c>
+      <c r="C12" s="41">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="D12" s="42">
+        <v>10</v>
+      </c>
+      <c r="E12" s="43">
+        <v>30</v>
+      </c>
+      <c r="F12" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="35"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="35"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="C13" s="41">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="D13" s="42">
+        <v>0</v>
+      </c>
+      <c r="E13" s="43">
+        <v>75</v>
+      </c>
+      <c r="F13" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="35"/>
+    </row>
+  </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;A</oddHeader>
     <oddFooter>Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1913,7 +3601,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1930,7 +3618,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1947,7 +3635,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1964,7 +3652,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1981,7 +3669,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1998,7 +3686,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2015,7 +3703,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
10.07 update by JUNKI LEE
</commit_message>
<xml_diff>
--- a/PSP_Sheet.xlsx
+++ b/PSP_Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Bigdata_Capstone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leejunki/Bigdata_Capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE850EE2-B21B-40EC-B185-302987568676}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A4D401-3B78-6948-B142-8DBBDB1BCB52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="432" yWindow="0" windowWidth="22608" windowHeight="12384" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="440" yWindow="460" windowWidth="22600" windowHeight="12380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="이준기" sheetId="1" r:id="rId1"/>
@@ -1175,7 +1175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
   <si>
     <t>Table C16  Time Recording Log</t>
   </si>
@@ -1323,286 +1323,169 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>주제</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>선정</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>및</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> skeleton code </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>작성자</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>선정</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>차</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>회의록</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>작성</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
       <t>9</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>월</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>월 19일</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="돋움"/>
+      <t xml:space="preserve"> 25</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Malgun Gothic"/>
         <family val="2"/>
         <charset val="129"/>
       </rPr>
-      <t>주제</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="돋움"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>선정</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="돋움"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>및</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> skeleton code </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="돋움"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>작성자</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="돋움"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>선정</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>9</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>월 20일</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Mission_0_template</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>작성 및 주제 구체화</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>9</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>월 23일</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="돋움"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>차</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="돋움"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>회의록</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="돋움"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>작성</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>9</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Malgun Gothic"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>월</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> 25</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Malgun Gothic"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
       <t>일</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>주제 수정 및 개선사항 점검</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">차 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="돋움"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>회의록</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="돋움"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>작성</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>9</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>월 30일</t>
     </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1756,29 +1639,6 @@
   </si>
   <si>
     <r>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>월 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="돋움"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>일</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">PPT </t>
     </r>
     <r>
@@ -1879,31 +1739,6 @@
   </si>
   <si>
     <r>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>월 1일</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>서베이 발표 및 GUI 디자인 회의, 요약본 요청</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t>9</t>
     </r>
     <r>
@@ -1936,126 +1771,54 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">PPT </t>
+      <t xml:space="preserve">2차 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>회의록</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="3"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
         <charset val="129"/>
       </rPr>
-      <t>추가</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
+      <t>작성</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>10월 1</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="10"/>
         <rFont val="돋움"/>
         <family val="2"/>
         <charset val="129"/>
       </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>작성</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="돋움"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>및</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="돋움"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>발표</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="돋움"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>초본</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="돋움"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>작성</t>
+      <t>일</t>
     </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <r>
-      <t>9</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>월</t>
+      <t>10</t>
     </r>
     <r>
       <rPr>
@@ -2063,64 +1826,37 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> 27</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="돋움"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>일</t>
+      <t>월 6일</t>
     </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">2차 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="돋움"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>회의록</t>
-    </r>
-    <r>
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="돋움"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>작성</t>
+      <t>분석 툴 선정 및 데이터 존재 확인, 질병 선택</t>
     </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <r>
-      <t>10월 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="돋움"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>일</t>
-    </r>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>월 7일</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>세부 질병 선택 및 질병 코드 확인 / 회의록 및 sheet 업데이트</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2132,7 +1868,7 @@
     <numFmt numFmtId="176" formatCode="m&quot;월&quot;\ d&quot;일&quot;;@"/>
     <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2203,11 +1939,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
@@ -2227,7 +1958,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -2287,6 +2018,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2295,7 +2037,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
@@ -2384,6 +2126,23 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="열어본 하이퍼링크" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -2769,20 +2528,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="11.5" style="8" customWidth="1"/>
     <col min="5" max="5" width="9.6640625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="46.44140625" customWidth="1"/>
+    <col min="6" max="6" width="46.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="11.7" customHeight="1">
+    <row r="1" spans="1:6" ht="11.75" customHeight="1">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -2794,10 +2553,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="11.7" customHeight="1">
+    <row r="2" spans="1:6" ht="11.75" customHeight="1">
       <c r="A2" s="20"/>
     </row>
-    <row r="3" spans="1:6" ht="11.7" customHeight="1">
+    <row r="3" spans="1:6" ht="11.75" customHeight="1">
       <c r="A3" s="19" t="s">
         <v>8</v>
       </c>
@@ -2807,8 +2566,8 @@
       </c>
       <c r="E3"/>
     </row>
-    <row r="4" spans="1:6" ht="11.7" customHeight="1"/>
-    <row r="5" spans="1:6" s="11" customFormat="1" ht="26.4">
+    <row r="4" spans="1:6" ht="11.75" customHeight="1"/>
+    <row r="5" spans="1:6" s="11" customFormat="1" ht="28">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
@@ -2989,20 +2748,44 @@
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="14"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="4"/>
+      <c r="A14" s="51" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D14" s="52">
+        <v>0</v>
+      </c>
+      <c r="E14" s="53">
+        <v>180</v>
+      </c>
+      <c r="F14" s="54" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1">
-      <c r="A15" s="14"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="4"/>
+      <c r="A15" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D15" s="52">
+        <v>60</v>
+      </c>
+      <c r="E15" s="53">
+        <v>300</v>
+      </c>
+      <c r="F15" s="54" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1">
       <c r="A16" s="14"/>
@@ -3205,7 +2988,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3222,7 +3005,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3239,7 +3022,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3256,7 +3039,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3273,7 +3056,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3290,7 +3073,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3307,7 +3090,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3320,13 +3103,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="13" t="s">
@@ -3345,7 +3128,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:11" ht="13.8">
+    <row r="3" spans="1:11" ht="14">
       <c r="A3" s="19" t="s">
         <v>8</v>
       </c>
@@ -3358,7 +3141,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:11" ht="26.4">
+    <row r="5" spans="1:11" ht="28">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
@@ -3383,7 +3166,7 @@
       <c r="J5" s="45"/>
       <c r="K5" s="45"/>
     </row>
-    <row r="6" spans="1:11" ht="13.8">
+    <row r="6" spans="1:11" ht="14">
       <c r="A6" s="30" t="s">
         <v>10</v>
       </c>
@@ -3400,7 +3183,7 @@
         <v>75</v>
       </c>
       <c r="F6" s="34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G6" s="35"/>
       <c r="H6" s="35"/>
@@ -3433,7 +3216,7 @@
       <c r="J7" s="35"/>
       <c r="K7" s="35"/>
     </row>
-    <row r="8" spans="1:11" ht="13.8">
+    <row r="8" spans="1:11" ht="14">
       <c r="A8" s="36" t="s">
         <v>14</v>
       </c>
@@ -3450,7 +3233,7 @@
         <v>30</v>
       </c>
       <c r="F8" s="40" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G8" s="35"/>
       <c r="H8" s="35"/>
@@ -3458,9 +3241,9 @@
       <c r="J8" s="35"/>
       <c r="K8" s="35"/>
     </row>
-    <row r="9" spans="1:11" ht="15.6">
+    <row r="9" spans="1:11" ht="15">
       <c r="A9" s="30" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B9" s="41">
         <v>0.41666666666666669</v>
@@ -3483,9 +3266,9 @@
       <c r="J9" s="35"/>
       <c r="K9" s="35"/>
     </row>
-    <row r="10" spans="1:11" ht="15.6">
+    <row r="10" spans="1:11" ht="15">
       <c r="A10" s="30" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B10" s="41">
         <v>0.16666666666666666</v>
@@ -3500,7 +3283,7 @@
         <v>30</v>
       </c>
       <c r="F10" s="44" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="G10" s="35"/>
       <c r="H10" s="35"/>
@@ -3508,7 +3291,7 @@
       <c r="J10" s="35"/>
       <c r="K10" s="35"/>
     </row>
-    <row r="11" spans="1:11" ht="15.6">
+    <row r="11" spans="1:11" ht="15">
       <c r="A11" s="30" t="s">
         <v>22</v>
       </c>
@@ -3525,7 +3308,7 @@
         <v>240</v>
       </c>
       <c r="F11" s="44" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="G11" s="35"/>
       <c r="H11" s="35"/>
@@ -3533,9 +3316,9 @@
       <c r="J11" s="35"/>
       <c r="K11" s="35"/>
     </row>
-    <row r="12" spans="1:11" ht="13.8">
+    <row r="12" spans="1:11" ht="14">
       <c r="A12" s="30" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B12" s="41">
         <v>0.4375</v>
@@ -3550,7 +3333,7 @@
         <v>30</v>
       </c>
       <c r="F12" s="44" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G12" s="35"/>
       <c r="H12" s="35"/>
@@ -3582,6 +3365,22 @@
       <c r="I13" s="35"/>
       <c r="J13" s="35"/>
       <c r="K13" s="35"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="46"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="50"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="46"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="50"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -3601,7 +3400,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3618,7 +3417,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3635,7 +3434,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3652,7 +3451,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3669,7 +3468,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3686,7 +3485,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3703,7 +3502,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
PSP, PMP, meeting report 10.12 update
</commit_message>
<xml_diff>
--- a/PSP_Sheet.xlsx
+++ b/PSP_Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Bigdata_Capstone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leejunki/Bigdata_Capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FBBB00-D1C4-4822-8671-FF1A4808EB01}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10ACF45-F518-0743-B1E6-E679EDA613FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="2880" windowWidth="21348" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="이준기" sheetId="1" r:id="rId1"/>
@@ -1175,7 +1175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
   <si>
     <t>Table C16  Time Recording Log</t>
   </si>
@@ -1912,6 +1912,22 @@
   </si>
   <si>
     <t>XD GUI 프로토타이핑</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>10월 10일</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data input, preprocessing, Modelling process Activity Diagram</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>10월 12일</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Activity Diagram 수정 및 비교분석 모델 선정</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2584,20 +2600,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="11.5" style="8" customWidth="1"/>
     <col min="5" max="5" width="9.6640625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="46.44140625" customWidth="1"/>
+    <col min="6" max="6" width="46.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="11.7" customHeight="1">
+    <row r="1" spans="1:6" ht="11.75" customHeight="1">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -2609,10 +2625,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="11.7" customHeight="1">
+    <row r="2" spans="1:6" ht="11.75" customHeight="1">
       <c r="A2" s="20"/>
     </row>
-    <row r="3" spans="1:6" ht="11.7" customHeight="1">
+    <row r="3" spans="1:6" ht="11.75" customHeight="1">
       <c r="A3" s="19" t="s">
         <v>8</v>
       </c>
@@ -2622,8 +2638,8 @@
       </c>
       <c r="E3"/>
     </row>
-    <row r="4" spans="1:6" ht="11.7" customHeight="1"/>
-    <row r="5" spans="1:6" s="11" customFormat="1" ht="26.4">
+    <row r="4" spans="1:6" ht="11.75" customHeight="1"/>
+    <row r="5" spans="1:6" s="11" customFormat="1" ht="28">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
@@ -2844,20 +2860,44 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1">
-      <c r="A16" s="14"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="4"/>
+      <c r="A16" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="D16" s="9">
+        <v>0</v>
+      </c>
+      <c r="E16" s="16">
+        <v>75</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1">
-      <c r="A17" s="14"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="4"/>
+      <c r="A17" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D17" s="9">
+        <v>60</v>
+      </c>
+      <c r="E17" s="16">
+        <v>240</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1">
       <c r="A18" s="14"/>
@@ -3044,7 +3084,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3061,7 +3101,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3078,7 +3118,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3095,7 +3135,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3112,7 +3152,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3129,7 +3169,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3146,7 +3186,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3161,11 +3201,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="13" t="s">
@@ -3184,7 +3224,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:11" ht="13.8">
+    <row r="3" spans="1:11" ht="14">
       <c r="A3" s="19" t="s">
         <v>8</v>
       </c>
@@ -3197,7 +3237,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:11" ht="26.4">
+    <row r="5" spans="1:11" ht="28">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
@@ -3222,7 +3262,7 @@
       <c r="J5" s="45"/>
       <c r="K5" s="45"/>
     </row>
-    <row r="6" spans="1:11" ht="13.8">
+    <row r="6" spans="1:11" ht="14">
       <c r="A6" s="30" t="s">
         <v>10</v>
       </c>
@@ -3272,7 +3312,7 @@
       <c r="J7" s="35"/>
       <c r="K7" s="35"/>
     </row>
-    <row r="8" spans="1:11" ht="13.8">
+    <row r="8" spans="1:11" ht="14">
       <c r="A8" s="36" t="s">
         <v>14</v>
       </c>
@@ -3297,7 +3337,7 @@
       <c r="J8" s="35"/>
       <c r="K8" s="35"/>
     </row>
-    <row r="9" spans="1:11" ht="15.6">
+    <row r="9" spans="1:11" ht="15">
       <c r="A9" s="30" t="s">
         <v>29</v>
       </c>
@@ -3322,7 +3362,7 @@
       <c r="J9" s="35"/>
       <c r="K9" s="35"/>
     </row>
-    <row r="10" spans="1:11" ht="15.6">
+    <row r="10" spans="1:11" ht="15">
       <c r="A10" s="30" t="s">
         <v>32</v>
       </c>
@@ -3347,7 +3387,7 @@
       <c r="J10" s="35"/>
       <c r="K10" s="35"/>
     </row>
-    <row r="11" spans="1:11" ht="15.6">
+    <row r="11" spans="1:11" ht="15">
       <c r="A11" s="30" t="s">
         <v>22</v>
       </c>
@@ -3372,7 +3412,7 @@
       <c r="J11" s="35"/>
       <c r="K11" s="35"/>
     </row>
-    <row r="12" spans="1:11" ht="13.8">
+    <row r="12" spans="1:11" ht="14">
       <c r="A12" s="30" t="s">
         <v>34</v>
       </c>
@@ -3422,7 +3462,7 @@
       <c r="J13" s="35"/>
       <c r="K13" s="35"/>
     </row>
-    <row r="14" spans="1:11" ht="15.6">
+    <row r="14" spans="1:11" ht="15">
       <c r="A14" s="46" t="s">
         <v>39</v>
       </c>
@@ -3442,7 +3482,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="13.8">
+    <row r="15" spans="1:11" ht="14">
       <c r="A15" s="46" t="s">
         <v>41</v>
       </c>
@@ -3480,7 +3520,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3497,7 +3537,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3514,7 +3554,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3531,7 +3571,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3548,7 +3588,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3565,7 +3605,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3582,7 +3622,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
PMP, PSP sheet update
</commit_message>
<xml_diff>
--- a/PSP_Sheet.xlsx
+++ b/PSP_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leejunki/Bigdata_Capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF963100-18C0-7444-9AFF-2F3D5A5D7A01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7B5777-F3B6-D747-8ECF-548E229761E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1175,7 +1175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
   <si>
     <t>Table C16  Time Recording Log</t>
   </si>
@@ -1960,6 +1960,14 @@
   </si>
   <si>
     <t>데이터 전처리 코딩 및 보건지수 다운로드</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>10월 29일</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Activity Diagram 전처리 파트 수정</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2633,7 +2641,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
@@ -3012,12 +3020,24 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1">
-      <c r="A22" s="14"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="4"/>
+      <c r="A22" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="D22" s="9">
+        <v>0</v>
+      </c>
+      <c r="E22" s="16">
+        <v>75</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="14"/>

</xml_diff>

<commit_message>
update report, PSP, django project file
</commit_message>
<xml_diff>
--- a/PSP_Sheet.xlsx
+++ b/PSP_Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Bigdata_Capstone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Bigdata_Capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1073CAB8-FF44-4AC8-AE8A-B363B3EEEB21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562C6524-31A0-4A23-9F30-5ADF9D074546}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9336" yWindow="0" windowWidth="11592" windowHeight="12384" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1380" yWindow="2880" windowWidth="21348" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="이준기" sheetId="1" r:id="rId1"/>
@@ -1175,7 +1175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="94">
   <si>
     <t>Table C16  Time Recording Log</t>
   </si>
@@ -2300,6 +2300,186 @@
         <charset val="129"/>
       </rPr>
       <t xml:space="preserve"> 기초 코드 실습</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>월 17</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Django Template 개발</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> 소스코드 Bootstrap 실습</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>월 21</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Diagram 피드백</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> 참여</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>월</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 27</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Django code, result page 캡쳐</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>, diagram upload</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>12월</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> 02일</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Django Chart 구현</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>12</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>월 03</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Django application 구현</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">, 보고서 수정, PSP sheet 수정 </t>
     </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -2988,7 +3168,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
@@ -3719,10 +3899,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
@@ -4220,6 +4400,106 @@
       </c>
       <c r="F25" s="58" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="13.8">
+      <c r="A26" s="59" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" s="47">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C26" s="47">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="D26" s="60">
+        <v>120</v>
+      </c>
+      <c r="E26" s="61">
+        <v>300</v>
+      </c>
+      <c r="F26" s="58" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="13.8">
+      <c r="A27" s="59" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="C27" s="47">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D27" s="60">
+        <v>0</v>
+      </c>
+      <c r="E27" s="61">
+        <v>60</v>
+      </c>
+      <c r="F27" s="58" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.6">
+      <c r="A28" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" s="47">
+        <v>0.625</v>
+      </c>
+      <c r="C28" s="47">
+        <v>0.75</v>
+      </c>
+      <c r="D28" s="60">
+        <v>30</v>
+      </c>
+      <c r="E28" s="61">
+        <v>150</v>
+      </c>
+      <c r="F28" s="58" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="13.8">
+      <c r="A29" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" s="47">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C29" s="47">
+        <v>1</v>
+      </c>
+      <c r="D29" s="60">
+        <v>20</v>
+      </c>
+      <c r="E29" s="61">
+        <v>100</v>
+      </c>
+      <c r="F29" s="58" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="13.8">
+      <c r="A30" s="59" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30" s="47">
+        <v>0</v>
+      </c>
+      <c r="C30" s="47">
+        <v>0.25</v>
+      </c>
+      <c r="D30" s="60">
+        <v>60</v>
+      </c>
+      <c r="E30" s="61">
+        <v>300</v>
+      </c>
+      <c r="F30" s="58" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>